<commit_message>
removed Medellin from notPresent dbs
</commit_message>
<xml_diff>
--- a/sui/data/energia/2021/2021_dbNotPresent.xlsx
+++ b/sui/data/energia/2021/2021_dbNotPresent.xlsx
@@ -1,21 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis documentos\JJ\repos\research_eslatina\sui\data\energia\2021\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="236" yWindow="13" windowWidth="16089" windowHeight="9661"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Municipio</t>
+  </si>
+  <si>
+    <t>CAUCA</t>
+  </si>
+  <si>
+    <t>TIMBIQUI</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,11 +85,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +139,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +171,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +206,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,47 +382,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Departamento</t>
-        </is>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Municipio</t>
-        </is>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ANTIOQUIA</t>
-        </is>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>MEDELLÍN</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CAUCA</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>TIMBIQUI</t>
-        </is>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>